<commit_message>
added optional arguments to script
</commit_message>
<xml_diff>
--- a/models/cluster/parameters.xlsx
+++ b/models/cluster/parameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>name</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>inverse</t>
+  </si>
+  <si>
+    <t>enabled</t>
   </si>
 </sst>
 </file>
@@ -384,7 +387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -465,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,28 +480,37 @@
     <col min="2" max="2" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>